<commit_message>
fixed typo in labels
</commit_message>
<xml_diff>
--- a/data/dictionary.xlsx
+++ b/data/dictionary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Lazaros\Project - 04 - AACN\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/07c4d937b78de3ca/R projects/AACN/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8937A0-871B-4560-9708-B4781EF531DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{4D8937A0-871B-4560-9708-B4781EF531DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D5C5EA5-34C9-4788-8896-97D0A27F19EA}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2217,8 +2217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fix label of moral_distress
</commit_message>
<xml_diff>
--- a/data/dictionary.xlsx
+++ b/data/dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/07c4d937b78de3ca/R projects/AACN/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{4D8937A0-871B-4560-9708-B4781EF531DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D5C5EA5-34C9-4788-8896-97D0A27F19EA}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{4D8937A0-871B-4560-9708-B4781EF531DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD5BF2FB-0EF7-4EA9-96DB-826EA3C80FFE}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="519">
   <si>
     <t>pos</t>
   </si>
@@ -447,9 +447,6 @@
   </si>
   <si>
     <t>C4</t>
-  </si>
-  <si>
-    <t>Moral distress has been defined as occurring when you know the appropriate action to take, but you are unable to act upon it and/or you act in a manner contrary to your personal and professional values, which undermines your integrity and authenticity. To what extent, in your work as a nurse do you experience moral distress?</t>
   </si>
   <si>
     <t>C5</t>
@@ -1609,6 +1606,12 @@
   </si>
   <si>
     <t>Recognition is most meaningful when it comes from:</t>
+  </si>
+  <si>
+    <t>To what extent, in your work as a nurse do you experience moral distress?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moral distress has been defined as occurring when you know the appropriate action to take, but you are unable to act upon it and/or you act in a manner contrary to your personal and professional values, which undermines your integrity and authenticity. </t>
   </si>
 </sst>
 </file>
@@ -2217,8 +2220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2236,16 +2239,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F1" s="9"/>
     </row>
@@ -2313,7 +2316,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -2327,7 +2330,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -2341,7 +2344,7 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
@@ -2355,7 +2358,7 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
@@ -2369,7 +2372,7 @@
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>
@@ -2481,7 +2484,7 @@
         <v>32</v>
       </c>
       <c r="C18" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D18" t="s">
         <v>33</v>
@@ -2554,10 +2557,10 @@
         <v>42</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="11"/>
@@ -2570,7 +2573,7 @@
         <v>43</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D24" t="s">
         <v>44</v>
@@ -2585,7 +2588,7 @@
         <v>45</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D25" t="s">
         <v>46</v>
@@ -2600,7 +2603,7 @@
         <v>47</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D26" t="s">
         <v>48</v>
@@ -2615,7 +2618,7 @@
         <v>49</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>50</v>
@@ -2630,7 +2633,7 @@
         <v>51</v>
       </c>
       <c r="C28" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D28" s="27" t="s">
         <v>52</v>
@@ -2645,7 +2648,7 @@
         <v>53</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D29" s="26" t="s">
         <v>54</v>
@@ -2660,7 +2663,7 @@
         <v>55</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D30" s="25" t="s">
         <v>56</v>
@@ -2675,7 +2678,7 @@
         <v>57</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D31" s="24" t="s">
         <v>58</v>
@@ -2690,7 +2693,7 @@
         <v>59</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D32" s="25" t="s">
         <v>60</v>
@@ -2705,7 +2708,7 @@
         <v>61</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D33" s="24" t="s">
         <v>62</v>
@@ -2720,7 +2723,7 @@
         <v>63</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D34" s="25" t="s">
         <v>64</v>
@@ -2735,7 +2738,7 @@
         <v>65</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D35" s="24" t="s">
         <v>66</v>
@@ -2750,7 +2753,7 @@
         <v>67</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D36" s="25" t="s">
         <v>68</v>
@@ -2765,7 +2768,7 @@
         <v>69</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D37" s="24" t="s">
         <v>70</v>
@@ -2780,7 +2783,7 @@
         <v>71</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D38" s="25" t="s">
         <v>72</v>
@@ -2795,7 +2798,7 @@
         <v>73</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D39" s="24" t="s">
         <v>74</v>
@@ -2810,7 +2813,7 @@
         <v>75</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D40" s="25" t="s">
         <v>76</v>
@@ -2825,7 +2828,7 @@
         <v>77</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D41" s="24" t="s">
         <v>78</v>
@@ -2840,7 +2843,7 @@
         <v>79</v>
       </c>
       <c r="C42" s="25" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D42" s="25" t="s">
         <v>80</v>
@@ -2855,7 +2858,7 @@
         <v>81</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D43" s="24" t="s">
         <v>82</v>
@@ -2870,7 +2873,7 @@
         <v>83</v>
       </c>
       <c r="C44" s="25" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D44" s="25" t="s">
         <v>84</v>
@@ -2885,7 +2888,7 @@
         <v>85</v>
       </c>
       <c r="C45" s="24" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D45" s="24" t="s">
         <v>86</v>
@@ -2900,7 +2903,7 @@
         <v>87</v>
       </c>
       <c r="C46" s="25" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D46" s="25" t="s">
         <v>88</v>
@@ -2915,7 +2918,7 @@
         <v>89</v>
       </c>
       <c r="C47" s="24" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D47" s="24" t="s">
         <v>90</v>
@@ -2930,7 +2933,7 @@
         <v>91</v>
       </c>
       <c r="C48" s="25" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D48" s="25" t="s">
         <v>92</v>
@@ -2945,7 +2948,7 @@
         <v>93</v>
       </c>
       <c r="C49" s="24" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D49" s="24" t="s">
         <v>94</v>
@@ -2960,7 +2963,7 @@
         <v>95</v>
       </c>
       <c r="C50" s="25" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D50" s="25" t="s">
         <v>96</v>
@@ -2975,7 +2978,7 @@
         <v>97</v>
       </c>
       <c r="C51" s="24" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D51" s="24" t="s">
         <v>98</v>
@@ -2990,7 +2993,7 @@
         <v>99</v>
       </c>
       <c r="C52" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D52" s="25" t="s">
         <v>100</v>
@@ -3005,7 +3008,7 @@
         <v>101</v>
       </c>
       <c r="C53" s="24" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D53" s="24" t="s">
         <v>102</v>
@@ -3020,7 +3023,7 @@
         <v>103</v>
       </c>
       <c r="C54" s="25" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D54" s="25" t="s">
         <v>104</v>
@@ -3035,7 +3038,7 @@
         <v>105</v>
       </c>
       <c r="C55" s="24" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D55" s="24" t="s">
         <v>106</v>
@@ -3050,7 +3053,7 @@
         <v>107</v>
       </c>
       <c r="C56" s="25" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D56" s="25" t="s">
         <v>108</v>
@@ -3065,7 +3068,7 @@
         <v>109</v>
       </c>
       <c r="C57" s="24" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D57" s="24" t="s">
         <v>110</v>
@@ -3080,7 +3083,7 @@
         <v>111</v>
       </c>
       <c r="C58" s="25" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D58" s="25" t="s">
         <v>112</v>
@@ -3095,7 +3098,7 @@
         <v>113</v>
       </c>
       <c r="C59" s="24" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D59" s="24" t="s">
         <v>114</v>
@@ -3110,7 +3113,7 @@
         <v>115</v>
       </c>
       <c r="C60" s="22" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D60" s="22" t="s">
         <v>116</v>
@@ -3125,13 +3128,13 @@
         <v>117</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D61" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="E61" s="3" t="s">
         <v>270</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>271</v>
       </c>
       <c r="F61" s="11"/>
     </row>
@@ -3143,10 +3146,10 @@
         <v>118</v>
       </c>
       <c r="C62" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D62" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -3157,10 +3160,10 @@
         <v>119</v>
       </c>
       <c r="C63" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D63" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -3171,10 +3174,10 @@
         <v>120</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3189,10 +3192,10 @@
         <v>collab_nurses</v>
       </c>
       <c r="D65" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -3207,7 +3210,7 @@
         <v>collab_physicians</v>
       </c>
       <c r="D66" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -3222,7 +3225,7 @@
         <v>collab_managers</v>
       </c>
       <c r="D67" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -3237,7 +3240,7 @@
         <v>collab_administration</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -3248,13 +3251,13 @@
         <v>125</v>
       </c>
       <c r="C69" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D69" t="s">
+        <v>278</v>
+      </c>
+      <c r="E69" s="3" t="s">
         <v>279</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3265,10 +3268,10 @@
         <v>126</v>
       </c>
       <c r="C70" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D70" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3279,10 +3282,10 @@
         <v>127</v>
       </c>
       <c r="C71" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D71" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3293,10 +3296,10 @@
         <v>128</v>
       </c>
       <c r="C72" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D72" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3307,13 +3310,13 @@
         <v>129</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -3321,10 +3324,13 @@
         <v>130</v>
       </c>
       <c r="C74" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>131</v>
+        <v>517</v>
+      </c>
+      <c r="E74" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3332,13 +3338,13 @@
         <v>74</v>
       </c>
       <c r="B75" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="D75" s="5" t="s">
         <v>132</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -3346,16 +3352,16 @@
         <v>75</v>
       </c>
       <c r="B76" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C76" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D76" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -3363,13 +3369,13 @@
         <v>76</v>
       </c>
       <c r="B77" s="34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C77" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D77" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -3377,13 +3383,13 @@
         <v>77</v>
       </c>
       <c r="B78" s="34" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C78" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D78" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -3391,13 +3397,13 @@
         <v>78</v>
       </c>
       <c r="B79" s="34" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C79" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D79" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -3405,13 +3411,13 @@
         <v>79</v>
       </c>
       <c r="B80" s="34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C80" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D80" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -3419,13 +3425,13 @@
         <v>80</v>
       </c>
       <c r="B81" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C81" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D81" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -3433,13 +3439,13 @@
         <v>81</v>
       </c>
       <c r="B82" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C82" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D82" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -3447,13 +3453,13 @@
         <v>82</v>
       </c>
       <c r="B83" s="34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C83" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D83" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3461,13 +3467,13 @@
         <v>83</v>
       </c>
       <c r="B84" s="34" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C84" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D84" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3475,13 +3481,13 @@
         <v>84</v>
       </c>
       <c r="B85" s="35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3489,17 +3495,17 @@
         <v>85</v>
       </c>
       <c r="B86" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C86" t="str">
         <f>SUBSTITUTE(C76,"mangr", "admin")</f>
         <v>admin_communication</v>
       </c>
       <c r="D86" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3507,14 +3513,14 @@
         <v>86</v>
       </c>
       <c r="B87" s="34" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C87" t="str">
         <f t="shared" ref="C87:C95" si="1">SUBSTITUTE(C77,"mangr", "admin")</f>
         <v>admin_collaboaration</v>
       </c>
       <c r="D87" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3522,14 +3528,14 @@
         <v>87</v>
       </c>
       <c r="B88" s="34" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C88" t="str">
         <f t="shared" si="1"/>
         <v>admin_staff</v>
       </c>
       <c r="D88" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -3537,14 +3543,14 @@
         <v>88</v>
       </c>
       <c r="B89" s="34" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C89" t="str">
         <f t="shared" si="1"/>
         <v>admin_supplies</v>
       </c>
       <c r="D89" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -3552,14 +3558,14 @@
         <v>89</v>
       </c>
       <c r="B90" s="34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C90" t="str">
         <f t="shared" si="1"/>
         <v>admin_decision</v>
       </c>
       <c r="D90" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3567,14 +3573,14 @@
         <v>90</v>
       </c>
       <c r="B91" s="34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C91" t="str">
         <f t="shared" si="1"/>
         <v>admin_recognition</v>
       </c>
       <c r="D91" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3582,14 +3588,14 @@
         <v>91</v>
       </c>
       <c r="B92" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C92" t="str">
         <f t="shared" si="1"/>
         <v>admin_leadership</v>
       </c>
       <c r="D92" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -3597,14 +3603,14 @@
         <v>92</v>
       </c>
       <c r="B93" s="34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="1"/>
         <v>admin_provision</v>
       </c>
       <c r="D93" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -3612,14 +3618,14 @@
         <v>93</v>
       </c>
       <c r="B94" s="34" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C94" t="str">
         <f t="shared" si="1"/>
         <v>admin_professional</v>
       </c>
       <c r="D94" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -3627,14 +3633,14 @@
         <v>94</v>
       </c>
       <c r="B95" s="35" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C95" s="5" t="str">
         <f t="shared" si="1"/>
         <v>admin_effectiveness</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -3642,13 +3648,13 @@
         <v>95</v>
       </c>
       <c r="B96" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="C96" t="s">
+        <v>376</v>
+      </c>
+      <c r="D96" t="s">
         <v>154</v>
-      </c>
-      <c r="C96" t="s">
-        <v>377</v>
-      </c>
-      <c r="D96" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -3656,13 +3662,13 @@
         <v>96</v>
       </c>
       <c r="B97" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="D97" s="5" t="s">
         <v>156</v>
-      </c>
-      <c r="C97" s="5" t="s">
-        <v>376</v>
-      </c>
-      <c r="D97" s="5" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -3670,16 +3676,16 @@
         <v>97</v>
       </c>
       <c r="B98" s="31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C98" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D98" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -3687,13 +3693,13 @@
         <v>98</v>
       </c>
       <c r="B99" s="31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C99" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D99" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -3701,13 +3707,13 @@
         <v>99</v>
       </c>
       <c r="B100" s="31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C100" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D100" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -3715,13 +3721,13 @@
         <v>100</v>
       </c>
       <c r="B101" s="31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C101" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D101" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -3729,13 +3735,13 @@
         <v>101</v>
       </c>
       <c r="B102" s="31" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C102" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D102" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -3743,13 +3749,13 @@
         <v>102</v>
       </c>
       <c r="B103" s="31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C103" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D103" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -3757,13 +3763,13 @@
         <v>103</v>
       </c>
       <c r="B104" s="31" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C104" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D104" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -3771,13 +3777,13 @@
         <v>104</v>
       </c>
       <c r="B105" s="31" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C105" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D105" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -3785,13 +3791,13 @@
         <v>105</v>
       </c>
       <c r="B106" s="31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C106" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D106" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -3799,13 +3805,13 @@
         <v>106</v>
       </c>
       <c r="B107" s="31" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C107" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D107" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -3813,13 +3819,13 @@
         <v>107</v>
       </c>
       <c r="B108" s="31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C108" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D108" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -3827,13 +3833,13 @@
         <v>108</v>
       </c>
       <c r="B109" s="31" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C109" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D109" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -3841,13 +3847,13 @@
         <v>109</v>
       </c>
       <c r="B110" s="31" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C110" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D110" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -3855,13 +3861,13 @@
         <v>110</v>
       </c>
       <c r="B111" s="31" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C111" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D111" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3869,13 +3875,13 @@
         <v>111</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -3883,16 +3889,16 @@
         <v>112</v>
       </c>
       <c r="B113" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C113" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D113" t="s">
+        <v>312</v>
+      </c>
+      <c r="E113" s="3" t="s">
         <v>313</v>
-      </c>
-      <c r="E113" s="3" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -3900,13 +3906,13 @@
         <v>113</v>
       </c>
       <c r="B114" s="29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C114" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D114" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E114" s="6"/>
       <c r="G114" s="3"/>
@@ -3916,13 +3922,13 @@
         <v>114</v>
       </c>
       <c r="B115" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C115" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D115" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E115" s="6"/>
       <c r="G115" s="3"/>
@@ -3932,13 +3938,13 @@
         <v>115</v>
       </c>
       <c r="B116" s="29" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C116" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D116" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E116" s="6"/>
       <c r="G116" s="3"/>
@@ -3948,13 +3954,13 @@
         <v>116</v>
       </c>
       <c r="B117" s="29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C117" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D117" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E117" s="6"/>
       <c r="G117" s="3"/>
@@ -3964,13 +3970,13 @@
         <v>117</v>
       </c>
       <c r="B118" s="30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E118" s="6"/>
       <c r="G118" s="3"/>
@@ -3980,13 +3986,13 @@
         <v>118</v>
       </c>
       <c r="B119" s="21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D119" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E119" s="6"/>
       <c r="G119" s="3"/>
@@ -3996,14 +4002,14 @@
         <v>119</v>
       </c>
       <c r="B120" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C120" t="str">
         <f>SUBSTITUTE(C113,"harass", "discrim")</f>
         <v>discrim_patients</v>
       </c>
       <c r="D120" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E120" s="6"/>
     </row>
@@ -4012,14 +4018,14 @@
         <v>120</v>
       </c>
       <c r="B121" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C121" t="str">
         <f t="shared" ref="C121:C126" si="2">SUBSTITUTE(C114,"harass", "discrim")</f>
         <v>discrim_families</v>
       </c>
       <c r="D121" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E121" s="6"/>
     </row>
@@ -4028,14 +4034,14 @@
         <v>121</v>
       </c>
       <c r="B122" s="29" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C122" t="str">
         <f t="shared" si="2"/>
         <v>discrim_nurse</v>
       </c>
       <c r="D122" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E122" s="6"/>
     </row>
@@ -4044,14 +4050,14 @@
         <v>122</v>
       </c>
       <c r="B123" s="29" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C123" t="str">
         <f t="shared" si="2"/>
         <v>discrim_physician</v>
       </c>
       <c r="D123" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E123" s="6"/>
     </row>
@@ -4060,14 +4066,14 @@
         <v>123</v>
       </c>
       <c r="B124" s="29" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C124" t="str">
         <f t="shared" si="2"/>
         <v>discrim_manager</v>
       </c>
       <c r="D124" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E124" s="6"/>
     </row>
@@ -4076,14 +4082,14 @@
         <v>124</v>
       </c>
       <c r="B125" s="30" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C125" t="str">
         <f t="shared" si="2"/>
         <v>discrim_administration</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E125" s="6"/>
     </row>
@@ -4092,14 +4098,14 @@
         <v>125</v>
       </c>
       <c r="B126" s="21" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C126" s="5" t="str">
         <f t="shared" si="2"/>
         <v>discrim_other</v>
       </c>
       <c r="D126" s="5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E126" s="6"/>
     </row>
@@ -4108,14 +4114,14 @@
         <v>126</v>
       </c>
       <c r="B127" s="29" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C127" t="str">
         <f>SUBSTITUTE(C120,"discrim", "abuse_verb")</f>
         <v>abuse_verb_patients</v>
       </c>
       <c r="D127" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E127" s="6"/>
     </row>
@@ -4124,14 +4130,14 @@
         <v>127</v>
       </c>
       <c r="B128" s="29" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C128" t="str">
         <f t="shared" ref="C128:C133" si="3">SUBSTITUTE(C121,"discrim", "abuse_verb")</f>
         <v>abuse_verb_families</v>
       </c>
       <c r="D128" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E128" s="6"/>
     </row>
@@ -4140,14 +4146,14 @@
         <v>128</v>
       </c>
       <c r="B129" s="29" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C129" t="str">
         <f t="shared" si="3"/>
         <v>abuse_verb_nurse</v>
       </c>
       <c r="D129" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E129" s="6"/>
     </row>
@@ -4156,14 +4162,14 @@
         <v>129</v>
       </c>
       <c r="B130" s="29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C130" t="str">
         <f t="shared" si="3"/>
         <v>abuse_verb_physician</v>
       </c>
       <c r="D130" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E130" s="6"/>
     </row>
@@ -4172,14 +4178,14 @@
         <v>130</v>
       </c>
       <c r="B131" s="30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C131" t="str">
         <f t="shared" si="3"/>
         <v>abuse_verb_manager</v>
       </c>
       <c r="D131" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E131" s="6"/>
     </row>
@@ -4188,14 +4194,14 @@
         <v>131</v>
       </c>
       <c r="B132" s="30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C132" t="str">
         <f t="shared" si="3"/>
         <v>abuse_verb_administration</v>
       </c>
       <c r="D132" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E132" s="6"/>
     </row>
@@ -4204,14 +4210,14 @@
         <v>132</v>
       </c>
       <c r="B133" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C133" s="5" t="str">
         <f t="shared" si="3"/>
         <v>abuse_verb_other</v>
       </c>
       <c r="D133" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E133" s="6"/>
     </row>
@@ -4220,14 +4226,14 @@
         <v>133</v>
       </c>
       <c r="B134" s="29" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C134" t="str">
         <f>SUBSTITUTE(C127,"abuse_verb", "abuse_phys")</f>
         <v>abuse_phys_patients</v>
       </c>
       <c r="D134" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E134" s="6"/>
     </row>
@@ -4236,14 +4242,14 @@
         <v>134</v>
       </c>
       <c r="B135" s="29" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C135" t="str">
         <f t="shared" ref="C135:C140" si="4">SUBSTITUTE(C128,"abuse_verb", "abuse_phys")</f>
         <v>abuse_phys_families</v>
       </c>
       <c r="D135" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E135" s="6"/>
     </row>
@@ -4252,14 +4258,14 @@
         <v>135</v>
       </c>
       <c r="B136" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C136" t="str">
         <f t="shared" si="4"/>
         <v>abuse_phys_nurse</v>
       </c>
       <c r="D136" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E136" s="6"/>
     </row>
@@ -4268,14 +4274,14 @@
         <v>136</v>
       </c>
       <c r="B137" s="29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C137" t="str">
         <f t="shared" si="4"/>
         <v>abuse_phys_physician</v>
       </c>
       <c r="D137" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E137" s="6"/>
     </row>
@@ -4284,14 +4290,14 @@
         <v>137</v>
       </c>
       <c r="B138" s="29" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C138" t="str">
         <f t="shared" si="4"/>
         <v>abuse_phys_manager</v>
       </c>
       <c r="D138" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E138" s="6"/>
     </row>
@@ -4300,14 +4306,14 @@
         <v>138</v>
       </c>
       <c r="B139" s="29" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C139" t="str">
         <f t="shared" si="4"/>
         <v>abuse_phys_administration</v>
       </c>
       <c r="D139" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E139" s="6"/>
     </row>
@@ -4316,14 +4322,14 @@
         <v>139</v>
       </c>
       <c r="B140" s="21" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C140" s="5" t="str">
         <f t="shared" si="4"/>
         <v>abuse_phys_other</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E140" s="6"/>
     </row>
@@ -4332,16 +4338,16 @@
         <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C141" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D141" t="s">
+        <v>429</v>
+      </c>
+      <c r="E141" s="3" t="s">
         <v>430</v>
-      </c>
-      <c r="E141" s="3" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -4349,13 +4355,13 @@
         <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C142" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D142" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -4363,13 +4369,13 @@
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C143" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D143" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -4377,13 +4383,13 @@
         <v>143</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D144" s="4" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -4391,13 +4397,13 @@
         <v>144</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D145" s="5" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -4405,13 +4411,13 @@
         <v>145</v>
       </c>
       <c r="B146" s="32" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C146" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D146" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -4419,13 +4425,13 @@
         <v>146</v>
       </c>
       <c r="B147" s="33" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D147" s="18" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E147" s="17"/>
     </row>
@@ -4434,16 +4440,16 @@
         <v>147</v>
       </c>
       <c r="B148" s="34" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C148" s="8" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D148" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E148" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -4451,13 +4457,13 @@
         <v>148</v>
       </c>
       <c r="B149" s="34" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C149" s="8" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D149" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -4465,13 +4471,13 @@
         <v>149</v>
       </c>
       <c r="B150" s="34" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C150" s="8" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D150" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -4479,13 +4485,13 @@
         <v>150</v>
       </c>
       <c r="B151" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C151" s="8" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D151" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E151" s="4"/>
     </row>
@@ -4494,13 +4500,13 @@
         <v>151</v>
       </c>
       <c r="B152" s="35" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C152" s="14" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D152" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E152" s="4"/>
     </row>
@@ -4509,13 +4515,13 @@
         <v>152</v>
       </c>
       <c r="B153" s="29" t="s">
+        <v>212</v>
+      </c>
+      <c r="C153" s="8" t="s">
+        <v>446</v>
+      </c>
+      <c r="D153" t="s">
         <v>213</v>
-      </c>
-      <c r="C153" s="8" t="s">
-        <v>447</v>
-      </c>
-      <c r="D153" t="s">
-        <v>214</v>
       </c>
       <c r="E153" s="4"/>
     </row>
@@ -4524,13 +4530,13 @@
         <v>153</v>
       </c>
       <c r="B154" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="C154" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="D154" t="s">
         <v>215</v>
-      </c>
-      <c r="C154" s="8" t="s">
-        <v>446</v>
-      </c>
-      <c r="D154" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -4538,13 +4544,13 @@
         <v>154</v>
       </c>
       <c r="B155" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="C155" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="D155" s="5" t="s">
         <v>217</v>
-      </c>
-      <c r="C155" s="5" t="s">
-        <v>409</v>
-      </c>
-      <c r="D155" s="5" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -4552,16 +4558,16 @@
         <v>155</v>
       </c>
       <c r="B156" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C156" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D156" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -4569,13 +4575,13 @@
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C157" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D157" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -4583,13 +4589,13 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C158" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D158" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -4597,13 +4603,13 @@
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C159" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D159" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -4611,13 +4617,13 @@
         <v>159</v>
       </c>
       <c r="B160" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C160" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D160" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -4625,13 +4631,13 @@
         <v>160</v>
       </c>
       <c r="B161" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C161" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D161" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -4639,13 +4645,13 @@
         <v>161</v>
       </c>
       <c r="B162" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C162" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D162" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -4653,13 +4659,13 @@
         <v>162</v>
       </c>
       <c r="B163" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C163" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D163" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -4667,13 +4673,13 @@
         <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C164" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D164" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -4681,13 +4687,13 @@
         <v>164</v>
       </c>
       <c r="B165" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C165" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D165" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -4695,13 +4701,13 @@
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C166" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D166" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -4709,13 +4715,13 @@
         <v>166</v>
       </c>
       <c r="B167" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C167" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D167" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -4723,13 +4729,13 @@
         <v>167</v>
       </c>
       <c r="B168" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D168" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E168" s="4"/>
     </row>
@@ -4738,13 +4744,13 @@
         <v>168</v>
       </c>
       <c r="B169" t="s">
+        <v>231</v>
+      </c>
+      <c r="C169" s="8" t="s">
+        <v>447</v>
+      </c>
+      <c r="D169" t="s">
         <v>232</v>
-      </c>
-      <c r="C169" s="8" t="s">
-        <v>448</v>
-      </c>
-      <c r="D169" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -4752,13 +4758,13 @@
         <v>169</v>
       </c>
       <c r="B170" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C170" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="D170" s="5" t="s">
         <v>234</v>
-      </c>
-      <c r="C170" s="5" t="s">
-        <v>449</v>
-      </c>
-      <c r="D170" s="5" t="s">
-        <v>235</v>
       </c>
       <c r="E170" s="4"/>
     </row>
@@ -4767,16 +4773,16 @@
         <v>170</v>
       </c>
       <c r="B171" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="C171" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="D171" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="C171" s="13" t="s">
-        <v>343</v>
-      </c>
-      <c r="D171" s="13" t="s">
-        <v>237</v>
-      </c>
       <c r="E171" s="16" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -4784,13 +4790,13 @@
         <v>171</v>
       </c>
       <c r="B172" t="s">
+        <v>237</v>
+      </c>
+      <c r="C172" t="s">
+        <v>343</v>
+      </c>
+      <c r="D172" t="s">
         <v>238</v>
-      </c>
-      <c r="C172" t="s">
-        <v>344</v>
-      </c>
-      <c r="D172" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -4798,13 +4804,13 @@
         <v>172</v>
       </c>
       <c r="B173" t="s">
+        <v>239</v>
+      </c>
+      <c r="C173" t="s">
+        <v>345</v>
+      </c>
+      <c r="D173" t="s">
         <v>240</v>
-      </c>
-      <c r="C173" t="s">
-        <v>346</v>
-      </c>
-      <c r="D173" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -4812,13 +4818,13 @@
         <v>173</v>
       </c>
       <c r="B174" t="s">
+        <v>241</v>
+      </c>
+      <c r="C174" t="s">
+        <v>344</v>
+      </c>
+      <c r="D174" t="s">
         <v>242</v>
-      </c>
-      <c r="C174" t="s">
-        <v>345</v>
-      </c>
-      <c r="D174" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
@@ -4826,13 +4832,13 @@
         <v>174</v>
       </c>
       <c r="B175" t="s">
+        <v>243</v>
+      </c>
+      <c r="C175" t="s">
+        <v>346</v>
+      </c>
+      <c r="D175" t="s">
         <v>244</v>
-      </c>
-      <c r="C175" t="s">
-        <v>347</v>
-      </c>
-      <c r="D175" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
@@ -4840,13 +4846,13 @@
         <v>175</v>
       </c>
       <c r="B176" t="s">
+        <v>245</v>
+      </c>
+      <c r="C176" t="s">
+        <v>347</v>
+      </c>
+      <c r="D176" t="s">
         <v>246</v>
-      </c>
-      <c r="C176" t="s">
-        <v>348</v>
-      </c>
-      <c r="D176" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -4854,13 +4860,13 @@
         <v>176</v>
       </c>
       <c r="B177" t="s">
+        <v>247</v>
+      </c>
+      <c r="C177" t="s">
+        <v>348</v>
+      </c>
+      <c r="D177" t="s">
         <v>248</v>
-      </c>
-      <c r="C177" t="s">
-        <v>349</v>
-      </c>
-      <c r="D177" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -4868,13 +4874,13 @@
         <v>177</v>
       </c>
       <c r="B178" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C178" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D178" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
@@ -4882,13 +4888,13 @@
         <v>178</v>
       </c>
       <c r="B179" t="s">
+        <v>250</v>
+      </c>
+      <c r="C179" t="s">
+        <v>350</v>
+      </c>
+      <c r="D179" t="s">
         <v>251</v>
-      </c>
-      <c r="C179" t="s">
-        <v>351</v>
-      </c>
-      <c r="D179" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
@@ -4896,13 +4902,13 @@
         <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C180" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D180" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
@@ -4910,13 +4916,13 @@
         <v>180</v>
       </c>
       <c r="B181" t="s">
+        <v>253</v>
+      </c>
+      <c r="C181" t="s">
+        <v>359</v>
+      </c>
+      <c r="D181" t="s">
         <v>254</v>
-      </c>
-      <c r="C181" t="s">
-        <v>360</v>
-      </c>
-      <c r="D181" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
@@ -4924,13 +4930,13 @@
         <v>181</v>
       </c>
       <c r="B182" t="s">
+        <v>255</v>
+      </c>
+      <c r="C182" t="s">
+        <v>352</v>
+      </c>
+      <c r="D182" t="s">
         <v>256</v>
-      </c>
-      <c r="C182" t="s">
-        <v>353</v>
-      </c>
-      <c r="D182" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
@@ -4938,13 +4944,13 @@
         <v>182</v>
       </c>
       <c r="B183" t="s">
+        <v>257</v>
+      </c>
+      <c r="C183" t="s">
+        <v>353</v>
+      </c>
+      <c r="D183" t="s">
         <v>258</v>
-      </c>
-      <c r="C183" t="s">
-        <v>354</v>
-      </c>
-      <c r="D183" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
@@ -4952,13 +4958,13 @@
         <v>183</v>
       </c>
       <c r="B184" t="s">
+        <v>259</v>
+      </c>
+      <c r="C184" t="s">
+        <v>356</v>
+      </c>
+      <c r="D184" t="s">
         <v>260</v>
-      </c>
-      <c r="C184" t="s">
-        <v>357</v>
-      </c>
-      <c r="D184" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -4966,13 +4972,13 @@
         <v>184</v>
       </c>
       <c r="B185" t="s">
+        <v>261</v>
+      </c>
+      <c r="C185" t="s">
+        <v>354</v>
+      </c>
+      <c r="D185" t="s">
         <v>262</v>
-      </c>
-      <c r="C185" t="s">
-        <v>355</v>
-      </c>
-      <c r="D185" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
@@ -4980,13 +4986,13 @@
         <v>185</v>
       </c>
       <c r="B186" t="s">
+        <v>263</v>
+      </c>
+      <c r="C186" t="s">
+        <v>355</v>
+      </c>
+      <c r="D186" t="s">
         <v>264</v>
-      </c>
-      <c r="C186" t="s">
-        <v>356</v>
-      </c>
-      <c r="D186" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
@@ -4994,13 +5000,13 @@
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C187" t="s">
+        <v>508</v>
+      </c>
+      <c r="D187" t="s">
         <v>509</v>
-      </c>
-      <c r="D187" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
@@ -5008,13 +5014,13 @@
         <v>187</v>
       </c>
       <c r="B188" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="C188" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="D188" s="15" t="s">
         <v>267</v>
-      </c>
-      <c r="C188" s="15" t="s">
-        <v>267</v>
-      </c>
-      <c r="D188" s="15" t="s">
-        <v>268</v>
       </c>
       <c r="E188" s="5"/>
     </row>
@@ -5053,13 +5059,13 @@
         <v>53</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C5" s="42" t="s">
         <v>54</v>
       </c>
       <c r="D5" s="43" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -5069,13 +5075,13 @@
         <v>57</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>58</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -5085,13 +5091,13 @@
         <v>61</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C7" s="38" t="s">
         <v>62</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -5101,13 +5107,13 @@
         <v>65</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C8" s="38" t="s">
         <v>66</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -5117,13 +5123,13 @@
         <v>69</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>70</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -5133,13 +5139,13 @@
         <v>73</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C10" s="38" t="s">
         <v>74</v>
       </c>
       <c r="D10" s="39" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -5149,13 +5155,13 @@
         <v>77</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C11" s="38" t="s">
         <v>78</v>
       </c>
       <c r="D11" s="39" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -5165,13 +5171,13 @@
         <v>81</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C12" s="38" t="s">
         <v>82</v>
       </c>
       <c r="D12" s="39" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -5181,13 +5187,13 @@
         <v>85</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>86</v>
       </c>
       <c r="D13" s="40" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -5197,13 +5203,13 @@
         <v>89</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C14" s="38" t="s">
         <v>90</v>
       </c>
       <c r="D14" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -5213,13 +5219,13 @@
         <v>93</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>94</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -5229,13 +5235,13 @@
         <v>97</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C16" s="38" t="s">
         <v>98</v>
       </c>
       <c r="D16" s="39" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -5245,13 +5251,13 @@
         <v>101</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>102</v>
       </c>
       <c r="D17" s="40" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
@@ -5261,13 +5267,13 @@
         <v>105</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C18" s="38" t="s">
         <v>106</v>
       </c>
       <c r="D18" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
@@ -5277,13 +5283,13 @@
         <v>109</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C19" s="38" t="s">
         <v>110</v>
       </c>
       <c r="D19" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -5293,13 +5299,13 @@
         <v>113</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C20" s="18" t="s">
         <v>114</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>

</xml_diff>